<commit_message>
object based sheet data
</commit_message>
<xml_diff>
--- a/operations.xlsx
+++ b/operations.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Number1</t>
+    <t>Number-1</t>
   </si>
   <si>
-    <t>Number2</t>
+    <t>Number-2</t>
   </si>
   <si>
     <t>Operation</t>

</xml_diff>